<commit_message>
Added utility functions and added missions to the spreadsheet
</commit_message>
<xml_diff>
--- a/Pokemon Black 2.xlsx
+++ b/Pokemon Black 2.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Areas" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Pokemon" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Missions" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="825">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -2473,6 +2474,30 @@
   </si>
   <si>
     <t xml:space="preserve">Genesect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Lost Boys!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collect Berries!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Audino!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The First Berry Search!</t>
   </si>
 </sst>
 </file>
@@ -2601,7 +2626,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2645,11 +2670,11 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.85"/>
@@ -2688,7 +2713,7 @@
       </c>
       <c r="E2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A2, ": { "," ""id"": 0x",A2,", ""key"": """,B2,""", ""display"": """,C2,""", ""prep"": """,D2,""", }, ")</f>
-        <v>0x1b6: {  "id": 0x1b6, "key": "AspertiaGate", "display": "the Aspertia Gate", "prep": "at", },</v>
+        <v>0x1b6: {  "id": 0x1b6, "key": "AspertiaGate", "display": "the Aspertia Gate", "prep": "at", }, </v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,7 +2731,7 @@
       </c>
       <c r="E3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A3, ": { "," ""id"": 0x",A3,", ""key"": """,B3,""", ""display"": """,C3,""", ""prep"": """,D3,""", }, ")</f>
-        <v>0x1b5: {  "id": 0x1b5, "key": "Route19", "display": "Route 19", "prep": "on", },</v>
+        <v>0x1b5: {  "id": 0x1b5, "key": "Route19", "display": "Route 19", "prep": "on", }, </v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,7 +2749,7 @@
       </c>
       <c r="E4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A4, ": { "," ""id"": 0x",A4,", ""key"": """,B4,""", ""display"": """,C4,""", ""prep"": """,D4,""", }, ")</f>
-        <v>0x1ab: {  "id": 0x1ab, "key": "Aspertia", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1ab: {  "id": 0x1ab, "key": "Aspertia", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2767,7 @@
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A5, ": { "," ""id"": 0x",A5,", ""key"": """,B5,""", ""display"": """,C5,""", ""prep"": """,D5,""", }, ")</f>
-        <v>0x1b1: {  "id": 0x1b1, "key": "AspertiaHouseTR1F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1b1: {  "id": 0x1b1, "key": "AspertiaHouseTR1F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2760,7 +2785,7 @@
       </c>
       <c r="E6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A6, ": { "," ""id"": 0x",A6,", ""key"": """,B6,""", ""display"": """,C6,""", ""prep"": """,D6,""", }, ")</f>
-        <v>0x1b2: {  "id": 0x1b2, "key": "AspertiaHouseTR2F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1b2: {  "id": 0x1b2, "key": "AspertiaHouseTR2F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,7 +2803,7 @@
       </c>
       <c r="E7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A7, ": { "," ""id"": 0x",A7,", ""key"": """,B7,""", ""display"": """,C7,""", ""prep"": """,D7,""", }, ")</f>
-        <v>0x1b3: {  "id": 0x1b3, "key": "AspertiaPokemonCenter", "display": "the Aspertia City Pokemon Center", "prep": "at", },</v>
+        <v>0x1b3: {  "id": 0x1b3, "key": "AspertiaPokemonCenter", "display": "the Aspertia City Pokemon Center", "prep": "at", }, </v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,7 +2821,7 @@
       </c>
       <c r="E8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A8, ": { "," ""id"": 0x",A8,", ""key"": """,B8,""", ""display"": """,C8,""", ""prep"": """,D8,""", }, ")</f>
-        <v>0x1ad: {  "id": 0x1ad, "key": "AspertiaHouseCL1F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1ad: {  "id": 0x1ad, "key": "AspertiaHouseCL1F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2814,7 +2839,7 @@
       </c>
       <c r="E9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A9, ": { "," ""id"": 0x",A9,", ""key"": """,B9,""", ""display"": """,C9,""", ""prep"": """,D9,""", }, ")</f>
-        <v>0x1ae: {  "id": 0x1ae, "key": "AspertiaHouseCL2F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1ae: {  "id": 0x1ae, "key": "AspertiaHouseCL2F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,7 +2857,7 @@
       </c>
       <c r="E10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A10, ": { "," ""id"": 0x",A10,", ""key"": """,B10,""", ""display"": """,C10,""", ""prep"": """,D10,""", }, ")</f>
-        <v>0x1af: {  "id": 0x1af, "key": "AspertiaHouseBL1F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1af: {  "id": 0x1af, "key": "AspertiaHouseBL1F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,7 +2875,7 @@
       </c>
       <c r="E11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A11, ": { "," ""id"": 0x",A11,", ""key"": """,B11,""", ""display"": """,C11,""", ""prep"": """,D11,""", }, ")</f>
-        <v>0x1b0: {  "id": 0x1b0, "key": "AspertiaHouseBL2F", "display": "Aspertia City", "prep": "in", },</v>
+        <v>0x1b0: {  "id": 0x1b0, "key": "AspertiaHouseBL2F", "display": "Aspertia City", "prep": "in", }, </v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,7 +2890,7 @@
       </c>
       <c r="E12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A12, ": { "," ""id"": 0x",A12,", ""key"": """,B12,""", ""display"": """,C12,""", ""prep"": """,D12,""", }, ")</f>
-        <v>0x1ac: {  "id": 0x1ac, "key": "PlayerHouse", "display": "home", "prep": "", },</v>
+        <v>0x1ac: {  "id": 0x1ac, "key": "PlayerHouse", "display": "home", "prep": "", }, </v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,7 +2908,7 @@
       </c>
       <c r="E13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A13, ": { "," ""id"": 0x",A13,", ""key"": """,B13,""", ""display"": """,C13,""", ""prep"": """,D13,""", }, ")</f>
-        <v>0x1b7: {  "id": 0x1b7, "key": "Floccesy", "display": "Floccesy Town", "prep": "in", },</v>
+        <v>0x1b7: {  "id": 0x1b7, "key": "Floccesy", "display": "Floccesy Town", "prep": "in", }, </v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,7 +2926,7 @@
       </c>
       <c r="E14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A14, ": { "," ""id"": 0x",A14,", ""key"": """,B14,""", ""display"": """,C14,""", ""prep"": """,D14,""", }, ")</f>
-        <v>0x1bb: {  "id": 0x1bb, "key": "FloccesyPokemonCenter", "display": "the Floccesy Town Pokemon Center", "prep": "at", },</v>
+        <v>0x1bb: {  "id": 0x1bb, "key": "FloccesyPokemonCenter", "display": "the Floccesy Town Pokemon Center", "prep": "at", }, </v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2919,7 +2944,7 @@
       </c>
       <c r="E15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A15, ": { "," ""id"": 0x",A15,", ""key"": """,B15,""", ""display"": """,C15,""", ""prep"": """,D15,""", }, ")</f>
-        <v>0x1b9: {  "id": 0x1b9, "key": "FloccesyHouseBC", "display": "Floccesy Town", "prep": "in", },</v>
+        <v>0x1b9: {  "id": 0x1b9, "key": "FloccesyHouseBC", "display": "Floccesy Town", "prep": "in", }, </v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,7 +2962,7 @@
       </c>
       <c r="E16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A16, ": { "," ""id"": 0x",A16,", ""key"": """,B16,""", ""display"": """,C16,""", ""prep"": """,D16,""", }, ")</f>
-        <v>0x1ba: {  "id": 0x1ba, "key": "FloccesyHouseBR", "display": "Floccesy Town", "prep": "in", },</v>
+        <v>0x1ba: {  "id": 0x1ba, "key": "FloccesyHouseBR", "display": "Floccesy Town", "prep": "in", }, </v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2955,7 +2980,7 @@
       </c>
       <c r="E17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A17, ": { "," ""id"": 0x",A17,", ""key"": """,B17,""", ""display"": """,C17,""", ""prep"": """,D17,""", }, ")</f>
-        <v>0x1be: {  "id": 0x1be, "key": "Route20", "display": "Route 20", "prep": "on", },</v>
+        <v>0x1be: {  "id": 0x1be, "key": "Route20", "display": "Route 20", "prep": "on", }, </v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2998,7 @@
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A18, ": { "," ""id"": 0x",A18,", ""key"": """,B18,""", ""display"": """,C18,""", ""prep"": """,D18,""", }, ")</f>
-        <v>0x1bc: {  "id": 0x1bc, "key": "Route20Ranch", "display": "Floccesy Ranch", "prep": "at", },</v>
+        <v>0x1bc: {  "id": 0x1bc, "key": "Route20Ranch", "display": "Floccesy Ranch", "prep": "at", }, </v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,7 +3016,7 @@
       </c>
       <c r="E19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A19, ": { "," ""id"": 0x",A19,", ""key"": """,B19,""", ""display"": """,C19,""", ""prep"": """,D19,""", }, ")</f>
-        <v>0x1bd: {  "id": 0x1bd, "key": "FloccesyRanch", "display": "Floccesy Ranch", "prep": "at", },</v>
+        <v>0x1bd: {  "id": 0x1bd, "key": "FloccesyRanch", "display": "Floccesy Ranch", "prep": "at", }, </v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,7 +3034,7 @@
       </c>
       <c r="E20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A20, ": { "," ""id"": 0x",A20,", ""key"": """,B20,""", ""display"": """,C20,""", ""prep"": """,D20,""", }, ")</f>
-        <v>0x1b8: {  "id": 0x1b8, "key": "FloccesyDojo", "display": "Floccesy Town", "prep": "in", },</v>
+        <v>0x1b8: {  "id": 0x1b8, "key": "FloccesyDojo", "display": "Floccesy Town", "prep": "in", }, </v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3027,7 +3052,7 @@
       </c>
       <c r="E21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A21, ": { "," ""id"": 0x",A21,", ""key"": """,B21,""", ""display"": """,C21,""", ""prep"": """,D21,""", }, ")</f>
-        <v>0x1b4: {  "id": 0x1b4, "key": "TrainerSchool", "display": "the Trainer School", "prep": "at", },</v>
+        <v>0x1b4: {  "id": 0x1b4, "key": "TrainerSchool", "display": "the Trainer School", "prep": "at", }, </v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3070,7 @@
       </c>
       <c r="E22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A22, ": { "," ""id"": 0x",A22,", ""key"": """,B22,""", ""display"": """,C22,""", ""prep"": """,D22,""", }, ")</f>
-        <v>0x1e9: {  "id": 0x1e9, "key": "AspertiaGym", "display": "the Aspertia City Gym", "prep": "at", },</v>
+        <v>0x1e9: {  "id": 0x1e9, "key": "AspertiaGym", "display": "the Aspertia City Gym", "prep": "at", }, </v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,109 +3220,109 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A31, ": { "," ""id"": 0x",A31,", ""key"": """,B31,""", ""display"": """,C31,""", ""prep"": """,D31,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A32, ": { "," ""id"": 0x",A32,", ""key"": """,B32,""", ""display"": """,C32,""", ""prep"": """,D32,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A33, ": { "," ""id"": 0x",A33,", ""key"": """,B33,""", ""display"": """,C33,""", ""prep"": """,D33,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A34, ": { "," ""id"": 0x",A34,", ""key"": """,B34,""", ""display"": """,C34,""", ""prep"": """,D34,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A35, ": { "," ""id"": 0x",A35,", ""key"": """,B35,""", ""display"": """,C35,""", ""prep"": """,D35,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A36, ": { "," ""id"": 0x",A36,", ""key"": """,B36,""", ""display"": """,C36,""", ""prep"": """,D36,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A37, ": { "," ""id"": 0x",A37,", ""key"": """,B37,""", ""display"": """,C37,""", ""prep"": """,D37,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A38, ": { "," ""id"": 0x",A38,", ""key"": """,B38,""", ""display"": """,C38,""", ""prep"": """,D38,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A39, ": { "," ""id"": 0x",A39,", ""key"": """,B39,""", ""display"": """,C39,""", ""prep"": """,D39,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A40, ": { "," ""id"": 0x",A40,", ""key"": """,B40,""", ""display"": """,C40,""", ""prep"": """,D40,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A41, ": { "," ""id"": 0x",A41,", ""key"": """,B41,""", ""display"": """,C41,""", ""prep"": """,D41,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A42, ": { "," ""id"": 0x",A42,", ""key"": """,B42,""", ""display"": """,C42,""", ""prep"": """,D42,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A43, ": { "," ""id"": 0x",A43,", ""key"": """,B43,""", ""display"": """,C43,""", ""prep"": """,D43,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A44, ": { "," ""id"": 0x",A44,", ""key"": """,B44,""", ""display"": """,C44,""", ""prep"": """,D44,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A45, ": { "," ""id"": 0x",A45,", ""key"": """,B45,""", ""display"": """,C45,""", ""prep"": """,D45,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A46, ": { "," ""id"": 0x",A46,", ""key"": """,B46,""", ""display"": """,C46,""", ""prep"": """,D46,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A47, ": { "," ""id"": 0x",A47,", ""key"": """,B47,""", ""display"": """,C47,""", ""prep"": """,D47,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("0x", A48, ": { "," ""id"": 0x",A48,", ""key"": """,B48,""", ""display"": """,C48,""", ""prep"": """,D48,""", }, ")</f>
-        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", },</v>
+        <v>0x: {  "id": 0x, "key": "", "display": "", "prep": "", }, </v>
       </c>
     </row>
   </sheetData>
@@ -3322,7 +3347,7 @@
       <selection pane="topLeft" activeCell="F650" activeCellId="0" sqref="F650"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.93"/>
@@ -16988,4 +17013,71 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>824</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>